<commit_message>
Created function to collect diff aggregation datatypes
</commit_message>
<xml_diff>
--- a/pm25year.xlsx
+++ b/pm25year.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,46 @@
           <t>value</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>q02</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>q25</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>median</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>q75</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>q98</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>avg</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -490,6 +530,30 @@
       <c r="F2" t="n">
         <v>7.83</v>
       </c>
+      <c r="G2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>4</v>
+      </c>
+      <c r="J2" t="n">
+        <v>7</v>
+      </c>
+      <c r="K2" t="n">
+        <v>10</v>
+      </c>
+      <c r="L2" t="n">
+        <v>21</v>
+      </c>
+      <c r="M2" t="n">
+        <v>44</v>
+      </c>
+      <c r="N2" t="n">
+        <v>7.829073905944824</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -516,6 +580,30 @@
       <c r="F3" t="n">
         <v>7.93</v>
       </c>
+      <c r="G3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J3" t="n">
+        <v>7</v>
+      </c>
+      <c r="K3" t="n">
+        <v>11</v>
+      </c>
+      <c r="L3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M3" t="n">
+        <v>36</v>
+      </c>
+      <c r="N3" t="n">
+        <v>7.932900428771973</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -542,6 +630,30 @@
       <c r="F4" t="n">
         <v>7.75</v>
       </c>
+      <c r="G4" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>4</v>
+      </c>
+      <c r="J4" t="n">
+        <v>7</v>
+      </c>
+      <c r="K4" t="n">
+        <v>11</v>
+      </c>
+      <c r="L4" t="n">
+        <v>22</v>
+      </c>
+      <c r="M4" t="n">
+        <v>50</v>
+      </c>
+      <c r="N4" t="n">
+        <v>7.747605800628662</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -568,6 +680,30 @@
       <c r="F5" t="n">
         <v>7.55</v>
       </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>4</v>
+      </c>
+      <c r="J5" t="n">
+        <v>6</v>
+      </c>
+      <c r="K5" t="n">
+        <v>10</v>
+      </c>
+      <c r="L5" t="n">
+        <v>22</v>
+      </c>
+      <c r="M5" t="n">
+        <v>49</v>
+      </c>
+      <c r="N5" t="n">
+        <v>7.5487380027771</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -594,6 +730,30 @@
       <c r="F6" t="n">
         <v>7.63</v>
       </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>4</v>
+      </c>
+      <c r="J6" t="n">
+        <v>7</v>
+      </c>
+      <c r="K6" t="n">
+        <v>10</v>
+      </c>
+      <c r="L6" t="n">
+        <v>22</v>
+      </c>
+      <c r="M6" t="n">
+        <v>80</v>
+      </c>
+      <c r="N6" t="n">
+        <v>7.633392810821533</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -620,6 +780,30 @@
       <c r="F7" t="n">
         <v>8.69</v>
       </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>5</v>
+      </c>
+      <c r="J7" t="n">
+        <v>8</v>
+      </c>
+      <c r="K7" t="n">
+        <v>11</v>
+      </c>
+      <c r="L7" t="n">
+        <v>23</v>
+      </c>
+      <c r="M7" t="n">
+        <v>52</v>
+      </c>
+      <c r="N7" t="n">
+        <v>8.692742347717285</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -646,6 +830,30 @@
       <c r="F8" t="n">
         <v>6.81</v>
       </c>
+      <c r="G8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>4</v>
+      </c>
+      <c r="J8" t="n">
+        <v>6</v>
+      </c>
+      <c r="K8" t="n">
+        <v>9</v>
+      </c>
+      <c r="L8" t="n">
+        <v>20</v>
+      </c>
+      <c r="M8" t="n">
+        <v>53</v>
+      </c>
+      <c r="N8" t="n">
+        <v>6.805400371551514</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -672,6 +880,30 @@
       <c r="F9" t="n">
         <v>7.96</v>
       </c>
+      <c r="G9" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>3</v>
+      </c>
+      <c r="J9" t="n">
+        <v>6</v>
+      </c>
+      <c r="K9" t="n">
+        <v>10</v>
+      </c>
+      <c r="L9" t="n">
+        <v>30.22000000000025</v>
+      </c>
+      <c r="M9" t="n">
+        <v>204</v>
+      </c>
+      <c r="N9" t="n">
+        <v>7.962154696132597</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -698,6 +930,30 @@
       <c r="F10" t="n">
         <v>7.24</v>
       </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>4</v>
+      </c>
+      <c r="J10" t="n">
+        <v>7</v>
+      </c>
+      <c r="K10" t="n">
+        <v>10</v>
+      </c>
+      <c r="L10" t="n">
+        <v>19</v>
+      </c>
+      <c r="M10" t="n">
+        <v>125</v>
+      </c>
+      <c r="N10" t="n">
+        <v>7.236739515652688</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -724,6 +980,30 @@
       <c r="F11" t="n">
         <v>7.1</v>
       </c>
+      <c r="G11" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I11" t="n">
+        <v>4</v>
+      </c>
+      <c r="J11" t="n">
+        <v>6</v>
+      </c>
+      <c r="K11" t="n">
+        <v>9</v>
+      </c>
+      <c r="L11" t="n">
+        <v>20</v>
+      </c>
+      <c r="M11" t="n">
+        <v>360</v>
+      </c>
+      <c r="N11" t="n">
+        <v>7.104579792256846</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -750,6 +1030,30 @@
       <c r="F12" t="n">
         <v>7.01</v>
       </c>
+      <c r="G12" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="I12" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="J12" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="K12" t="n">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="L12" t="n">
+        <v>21.8</v>
+      </c>
+      <c r="M12" t="n">
+        <v>137.8</v>
+      </c>
+      <c r="N12" t="n">
+        <v>7.007795536791313</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -776,6 +1080,30 @@
       <c r="F13" t="n">
         <v>7.9</v>
       </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>4</v>
+      </c>
+      <c r="J13" t="n">
+        <v>7</v>
+      </c>
+      <c r="K13" t="n">
+        <v>10</v>
+      </c>
+      <c r="L13" t="n">
+        <v>22</v>
+      </c>
+      <c r="M13" t="n">
+        <v>54</v>
+      </c>
+      <c r="N13" t="n">
+        <v>7.904960632324219</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -802,6 +1130,30 @@
       <c r="F14" t="n">
         <v>8.09</v>
       </c>
+      <c r="G14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="n">
+        <v>5</v>
+      </c>
+      <c r="J14" t="n">
+        <v>7</v>
+      </c>
+      <c r="K14" t="n">
+        <v>11</v>
+      </c>
+      <c r="L14" t="n">
+        <v>21</v>
+      </c>
+      <c r="M14" t="n">
+        <v>78</v>
+      </c>
+      <c r="N14" t="n">
+        <v>8.091594696044922</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -828,6 +1180,30 @@
       <c r="F15" t="n">
         <v>9.65</v>
       </c>
+      <c r="G15" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" t="n">
+        <v>6</v>
+      </c>
+      <c r="J15" t="n">
+        <v>9</v>
+      </c>
+      <c r="K15" t="n">
+        <v>13</v>
+      </c>
+      <c r="L15" t="n">
+        <v>24</v>
+      </c>
+      <c r="M15" t="n">
+        <v>69</v>
+      </c>
+      <c r="N15" t="n">
+        <v>9.649613380432129</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -854,6 +1230,30 @@
       <c r="F16" t="n">
         <v>8.49</v>
       </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>5</v>
+      </c>
+      <c r="J16" t="n">
+        <v>7</v>
+      </c>
+      <c r="K16" t="n">
+        <v>11</v>
+      </c>
+      <c r="L16" t="n">
+        <v>25</v>
+      </c>
+      <c r="M16" t="n">
+        <v>53</v>
+      </c>
+      <c r="N16" t="n">
+        <v>8.487636566162109</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -880,6 +1280,30 @@
       <c r="F17" t="n">
         <v>5.9</v>
       </c>
+      <c r="G17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I17" t="n">
+        <v>3</v>
+      </c>
+      <c r="J17" t="n">
+        <v>5</v>
+      </c>
+      <c r="K17" t="n">
+        <v>8</v>
+      </c>
+      <c r="L17" t="n">
+        <v>20</v>
+      </c>
+      <c r="M17" t="n">
+        <v>69</v>
+      </c>
+      <c r="N17" t="n">
+        <v>5.902006149291992</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -906,6 +1330,30 @@
       <c r="F18" t="n">
         <v>7.55</v>
       </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>4</v>
+      </c>
+      <c r="J18" t="n">
+        <v>7</v>
+      </c>
+      <c r="K18" t="n">
+        <v>10</v>
+      </c>
+      <c r="L18" t="n">
+        <v>21</v>
+      </c>
+      <c r="M18" t="n">
+        <v>52</v>
+      </c>
+      <c r="N18" t="n">
+        <v>7.549196720123291</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -932,6 +1380,30 @@
       <c r="F19" t="n">
         <v>10.2</v>
       </c>
+      <c r="G19" t="n">
+        <v>2</v>
+      </c>
+      <c r="H19" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" t="n">
+        <v>5</v>
+      </c>
+      <c r="J19" t="n">
+        <v>9</v>
+      </c>
+      <c r="K19" t="n">
+        <v>14</v>
+      </c>
+      <c r="L19" t="n">
+        <v>24.45999908447266</v>
+      </c>
+      <c r="M19" t="n">
+        <v>40</v>
+      </c>
+      <c r="N19" t="n">
+        <v>10.21666622161865</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -958,6 +1430,30 @@
       <c r="F20" t="n">
         <v>6.96</v>
       </c>
+      <c r="G20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>3</v>
+      </c>
+      <c r="J20" t="n">
+        <v>6</v>
+      </c>
+      <c r="K20" t="n">
+        <v>10</v>
+      </c>
+      <c r="L20" t="n">
+        <v>20</v>
+      </c>
+      <c r="M20" t="n">
+        <v>62</v>
+      </c>
+      <c r="N20" t="n">
+        <v>6.956928253173828</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -984,6 +1480,30 @@
       <c r="F21" t="n">
         <v>8.66</v>
       </c>
+      <c r="G21" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H21" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>4</v>
+      </c>
+      <c r="J21" t="n">
+        <v>6</v>
+      </c>
+      <c r="K21" t="n">
+        <v>10</v>
+      </c>
+      <c r="L21" t="n">
+        <v>33</v>
+      </c>
+      <c r="M21" t="n">
+        <v>244</v>
+      </c>
+      <c r="N21" t="n">
+        <v>8.657696597880648</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1010,6 +1530,30 @@
       <c r="F22" t="n">
         <v>6.69</v>
       </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>3</v>
+      </c>
+      <c r="J22" t="n">
+        <v>6</v>
+      </c>
+      <c r="K22" t="n">
+        <v>9</v>
+      </c>
+      <c r="L22" t="n">
+        <v>19</v>
+      </c>
+      <c r="M22" t="n">
+        <v>85</v>
+      </c>
+      <c r="N22" t="n">
+        <v>6.686489058039962</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1036,6 +1580,30 @@
       <c r="F23" t="n">
         <v>7.69</v>
       </c>
+      <c r="G23" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1</v>
+      </c>
+      <c r="I23" t="n">
+        <v>4</v>
+      </c>
+      <c r="J23" t="n">
+        <v>7</v>
+      </c>
+      <c r="K23" t="n">
+        <v>10</v>
+      </c>
+      <c r="L23" t="n">
+        <v>20</v>
+      </c>
+      <c r="M23" t="n">
+        <v>131</v>
+      </c>
+      <c r="N23" t="n">
+        <v>7.690385530699666</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1062,6 +1630,30 @@
       <c r="F24" t="n">
         <v>8.93</v>
       </c>
+      <c r="G24" t="n">
+        <v>2.8512</v>
+      </c>
+      <c r="H24" t="n">
+        <v>2.8512</v>
+      </c>
+      <c r="I24" t="n">
+        <v>5.03</v>
+      </c>
+      <c r="J24" t="n">
+        <v>7.117083333333333</v>
+      </c>
+      <c r="K24" t="n">
+        <v>10.47625</v>
+      </c>
+      <c r="L24" t="n">
+        <v>26.44700000000003</v>
+      </c>
+      <c r="M24" t="n">
+        <v>175.495</v>
+      </c>
+      <c r="N24" t="n">
+        <v>8.931984381063245</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1088,6 +1680,30 @@
       <c r="F25" t="n">
         <v>12.7</v>
       </c>
+      <c r="G25" t="n">
+        <v>0.9615833379576604</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.9615833379576604</v>
+      </c>
+      <c r="I25" t="n">
+        <v>4.528125002980232</v>
+      </c>
+      <c r="J25" t="n">
+        <v>9.709750016530354</v>
+      </c>
+      <c r="K25" t="n">
+        <v>16.31174997488658</v>
+      </c>
+      <c r="L25" t="n">
+        <v>43.18033254623413</v>
+      </c>
+      <c r="M25" t="n">
+        <v>202.4250005086263</v>
+      </c>
+      <c r="N25" t="n">
+        <v>12.6525999722694</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1114,6 +1730,30 @@
       <c r="F26" t="n">
         <v>12.7</v>
       </c>
+      <c r="G26" t="n">
+        <v>0.7065541703402995</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.7065541703402995</v>
+      </c>
+      <c r="I26" t="n">
+        <v>4.619281297922134</v>
+      </c>
+      <c r="J26" t="n">
+        <v>9.706145902474722</v>
+      </c>
+      <c r="K26" t="n">
+        <v>18.08900010585785</v>
+      </c>
+      <c r="L26" t="n">
+        <v>38.98978563308715</v>
+      </c>
+      <c r="M26" t="n">
+        <v>148.2515411376953</v>
+      </c>
+      <c r="N26" t="n">
+        <v>12.66643034488212</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1140,6 +1780,30 @@
       <c r="F27" t="n">
         <v>14.9</v>
       </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>3.355833331743876</v>
+      </c>
+      <c r="J27" t="n">
+        <v>7.675625006357829</v>
+      </c>
+      <c r="K27" t="n">
+        <v>26.57737493515015</v>
+      </c>
+      <c r="L27" t="n">
+        <v>47.48729972839356</v>
+      </c>
+      <c r="M27" t="n">
+        <v>96.08124923706055</v>
+      </c>
+      <c r="N27" t="n">
+        <v>14.88347807317683</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1165,6 +1829,30 @@
       </c>
       <c r="F28" t="n">
         <v>10.1</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.8354166708886623</v>
+      </c>
+      <c r="J28" t="n">
+        <v>5.08216667175293</v>
+      </c>
+      <c r="K28" t="n">
+        <v>15.78683334986369</v>
+      </c>
+      <c r="L28" t="n">
+        <v>41.69837659200033</v>
+      </c>
+      <c r="M28" t="n">
+        <v>221.996084416906</v>
+      </c>
+      <c r="N28" t="n">
+        <v>10.12769062769757</v>
       </c>
     </row>
   </sheetData>

</xml_diff>